<commit_message>
fix tests and add table
</commit_message>
<xml_diff>
--- a/benchmark.xlsx
+++ b/benchmark.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\permi\source\repos\university\da\2_dict\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7655D18-D594-47EC-9A19-214A8F60F444}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E646B542-CDA9-499E-A315-F96FCAEA780F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{1FD290DD-753F-4FFC-B3B8-1A81E5A9B584}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11505" xr2:uid="{1FD290DD-753F-4FFC-B3B8-1A81E5A9B584}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -414,7 +414,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,10 +454,10 @@
         <v>200</v>
       </c>
       <c r="C3">
-        <v>350.07459999999998</v>
+        <v>16.847999999999999</v>
       </c>
       <c r="D3">
-        <v>350.07799999999997</v>
+        <v>159.078</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -468,10 +468,10 @@
         <v>1000</v>
       </c>
       <c r="C4">
-        <v>367.46210000000002</v>
+        <v>18.535</v>
       </c>
       <c r="D4">
-        <v>361.44299999999998</v>
+        <v>186.143</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -482,10 +482,10 @@
         <v>10000</v>
       </c>
       <c r="C5">
-        <v>399.61529999999999</v>
+        <v>25.616</v>
       </c>
       <c r="D5">
-        <v>371.14299999999997</v>
+        <v>247.488</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -496,10 +496,10 @@
         <v>100000</v>
       </c>
       <c r="C6">
-        <v>427.21420000000001</v>
+        <v>43.213999999999999</v>
       </c>
       <c r="D6">
-        <v>375.721</v>
+        <v>326.721</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -510,10 +510,10 @@
         <v>1000000</v>
       </c>
       <c r="C7">
-        <v>439.01749999999998</v>
+        <v>71.015000000000001</v>
       </c>
       <c r="D7">
-        <v>382.76900000000001</v>
+        <v>376.96899999999999</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -554,10 +554,10 @@
         <v>200</v>
       </c>
       <c r="C11">
-        <v>515.20500000000004</v>
+        <v>126.142</v>
       </c>
       <c r="D11">
-        <v>441.03800000000001</v>
+        <v>160.54499999999999</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -568,10 +568,10 @@
         <v>1000</v>
       </c>
       <c r="C12">
-        <v>536.42970000000003</v>
+        <v>165.85900000000001</v>
       </c>
       <c r="D12">
-        <v>446.80500000000001</v>
+        <v>198.40299999999999</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -582,10 +582,10 @@
         <v>10000</v>
       </c>
       <c r="C13">
-        <v>583.40120000000002</v>
+        <v>264.42599999999999</v>
       </c>
       <c r="D13">
-        <v>452.19600000000003</v>
+        <v>273.97300000000001</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -596,10 +596,10 @@
         <v>100000</v>
       </c>
       <c r="C14">
-        <v>665.69370000000004</v>
+        <v>370.57</v>
       </c>
       <c r="D14">
-        <v>466.98399999999998</v>
+        <v>345.28899999999999</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -610,10 +610,10 @@
         <v>1000000</v>
       </c>
       <c r="C15">
-        <v>774.86630000000002</v>
+        <v>439.923</v>
       </c>
       <c r="D15">
-        <v>469.48200000000003</v>
+        <v>419.65300000000002</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -654,10 +654,10 @@
         <v>200</v>
       </c>
       <c r="C19">
-        <v>487.98200000000003</v>
+        <v>557.98199999999997</v>
       </c>
       <c r="D19">
-        <v>466.01100000000002</v>
+        <v>646.01099999999997</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -668,10 +668,10 @@
         <v>1000</v>
       </c>
       <c r="C20">
-        <v>506.09039999999999</v>
+        <v>576.09400000000005</v>
       </c>
       <c r="D20">
-        <v>462.21800000000002</v>
+        <v>692.21799999999996</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -682,10 +682,10 @@
         <v>10000</v>
       </c>
       <c r="C21">
-        <v>597.72820000000002</v>
+        <v>657.28200000000004</v>
       </c>
       <c r="D21">
-        <v>483.45400000000001</v>
+        <v>783.45399999999995</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -696,10 +696,10 @@
         <v>100000</v>
       </c>
       <c r="C22">
-        <v>690.43320000000006</v>
+        <v>790.43200000000002</v>
       </c>
       <c r="D22">
-        <v>487.25900000000001</v>
+        <v>917.25900000000001</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -710,10 +710,10 @@
         <v>1000000</v>
       </c>
       <c r="C23">
-        <v>822.83370000000002</v>
+        <v>872.33699999999999</v>
       </c>
       <c r="D23">
-        <v>491.43200000000002</v>
+        <v>1011.432</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix tests and calc in table
</commit_message>
<xml_diff>
--- a/benchmark.xlsx
+++ b/benchmark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\permi\source\repos\university\da\2_dict\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E646B542-CDA9-499E-A315-F96FCAEA780F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8DE002-4287-497D-8539-5AA9A6522A1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11505" xr2:uid="{1FD290DD-753F-4FFC-B3B8-1A81E5A9B584}"/>
   </bookViews>
@@ -414,7 +414,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,10 +454,10 @@
         <v>200</v>
       </c>
       <c r="C3">
-        <v>16.847999999999999</v>
+        <v>1.6E-2</v>
       </c>
       <c r="D3">
-        <v>159.078</v>
+        <v>2.7E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -468,10 +468,10 @@
         <v>1000</v>
       </c>
       <c r="C4">
-        <v>18.535</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="D4">
-        <v>186.143</v>
+        <v>0.186</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -482,10 +482,10 @@
         <v>10000</v>
       </c>
       <c r="C5">
-        <v>25.616</v>
+        <v>2.9609999999999999</v>
       </c>
       <c r="D5">
-        <v>247.488</v>
+        <v>4.4880000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -496,10 +496,10 @@
         <v>100000</v>
       </c>
       <c r="C6">
-        <v>43.213999999999999</v>
+        <v>46.213999999999999</v>
       </c>
       <c r="D6">
-        <v>326.721</v>
+        <v>63.720999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -510,10 +510,10 @@
         <v>1000000</v>
       </c>
       <c r="C7">
-        <v>71.015000000000001</v>
+        <v>971.01499999999999</v>
       </c>
       <c r="D7">
-        <v>376.96899999999999</v>
+        <v>1076.9690000000001</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -554,10 +554,10 @@
         <v>200</v>
       </c>
       <c r="C11">
-        <v>126.142</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="D11">
-        <v>160.54499999999999</v>
+        <v>0.245</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -568,10 +568,10 @@
         <v>1000</v>
       </c>
       <c r="C12">
-        <v>165.85900000000001</v>
+        <v>0.45900000000000002</v>
       </c>
       <c r="D12">
-        <v>198.40299999999999</v>
+        <v>0.503</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -582,10 +582,10 @@
         <v>10000</v>
       </c>
       <c r="C13">
-        <v>264.42599999999999</v>
+        <v>4.4260000000000002</v>
       </c>
       <c r="D13">
-        <v>273.97300000000001</v>
+        <v>4.0730000000000004</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -596,10 +596,10 @@
         <v>100000</v>
       </c>
       <c r="C14">
-        <v>370.57</v>
+        <v>60.356999999999999</v>
       </c>
       <c r="D14">
-        <v>345.28899999999999</v>
+        <v>45.289000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -610,10 +610,10 @@
         <v>1000000</v>
       </c>
       <c r="C15">
-        <v>439.923</v>
+        <v>1239.923</v>
       </c>
       <c r="D15">
-        <v>419.65300000000002</v>
+        <v>990.65300000000002</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -654,10 +654,10 @@
         <v>200</v>
       </c>
       <c r="C19">
-        <v>557.98199999999997</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="D19">
-        <v>646.01099999999997</v>
+        <v>5.5E-2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -668,10 +668,10 @@
         <v>1000</v>
       </c>
       <c r="C20">
-        <v>576.09400000000005</v>
+        <v>0.254</v>
       </c>
       <c r="D20">
-        <v>692.21799999999996</v>
+        <v>0.38600000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -682,10 +682,10 @@
         <v>10000</v>
       </c>
       <c r="C21">
-        <v>657.28200000000004</v>
+        <v>3.282</v>
       </c>
       <c r="D21">
-        <v>783.45399999999995</v>
+        <v>3.6539999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -696,10 +696,10 @@
         <v>100000</v>
       </c>
       <c r="C22">
-        <v>790.43200000000002</v>
+        <v>68.432000000000002</v>
       </c>
       <c r="D22">
-        <v>917.25900000000001</v>
+        <v>59.259</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -710,10 +710,10 @@
         <v>1000000</v>
       </c>
       <c r="C23">
-        <v>872.33699999999999</v>
+        <v>1465.337</v>
       </c>
       <c r="D23">
-        <v>1011.432</v>
+        <v>1270.432</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>